<commit_message>
added charts in csv
</commit_message>
<xml_diff>
--- a/Aufgabe 3/TCP/TCP_benchmarking_csv.xlsx
+++ b/Aufgabe 3/TCP/TCP_benchmarking_csv.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonsymhoven/Desktop/Uni/FHAW/WS_2019_2020/Datenkommunikation/Datenkommunikation/Aufgabe 3/TCP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F590252-0103-5648-B804-6B581797AA9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB780BDF-5E50-B145-8BBC-EDAE9C811E1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2480" yWindow="1220" windowWidth="20420" windowHeight="12980" xr2:uid="{5A66E864-9B9D-D645-9740-394DE20EA0D4}"/>
+    <workbookView xWindow="2480" yWindow="1220" windowWidth="20420" windowHeight="12980" activeTab="1" xr2:uid="{5A66E864-9B9D-D645-9740-394DE20EA0D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="81">
   <si>
     <t>Messungstyp als String</t>
   </si>
@@ -309,8 +313,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -326,6 +337,1197 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Median</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>20</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>30</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>40</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Sheet1!$G$7,Sheet1!$G$13,Sheet1!$G$19,Sheet1!$G$25,Sheet1!$G$31)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.9579999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.702</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.1219999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.1440000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.215999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-49EA-E843-BCC9-FF86001467BC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>RTT</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>20</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>30</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>40</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Sheet1!$N$7,Sheet1!$N$13,Sheet1!$N$19,Sheet1!$N$25,Sheet1!$N$31)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.0540000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.58</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.731999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.032000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.663999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-49EA-E843-BCC9-FF86001467BC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1019135072"/>
+        <c:axId val="1019112000"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1019135072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Anzahl</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1019112000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1019112000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="25"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Zeit</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> in ms</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1019135072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BDAB8DA-1567-524F-9C3E-3DB4DF81CB77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -625,13 +1827,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3CC8E52-2AD3-0945-9A75-C519621EDCC5}">
-  <dimension ref="A1:AC26"/>
+  <dimension ref="A1:AC31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="L10" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="48.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="57.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="46.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="66" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="54.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="74" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="43" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="44.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -723,16 +1951,16 @@
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>20</v>
       </c>
       <c r="E2">
@@ -812,18 +2040,10 @@
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
       <c r="E3">
         <v>2.4500000000000002</v>
       </c>
@@ -901,18 +2121,10 @@
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>20</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="E4">
         <v>2.3199999999999998</v>
       </c>
@@ -990,18 +2202,10 @@
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
-      <c r="D5">
-        <v>20</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
       <c r="E5">
         <v>2.58</v>
       </c>
@@ -1079,18 +2283,10 @@
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <v>20</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
       <c r="E6">
         <v>2.46</v>
       </c>
@@ -1168,142 +2364,67 @@
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>20</v>
-      </c>
-      <c r="D7">
-        <v>20</v>
-      </c>
-      <c r="E7">
-        <v>3.55</v>
-      </c>
-      <c r="F7">
-        <v>3.76</v>
-      </c>
-      <c r="G7">
-        <v>4.8</v>
-      </c>
-      <c r="H7">
-        <v>6.99</v>
-      </c>
-      <c r="I7">
-        <v>15.32</v>
-      </c>
-      <c r="J7">
-        <v>64.97</v>
-      </c>
-      <c r="K7">
-        <v>3.23</v>
-      </c>
-      <c r="L7">
-        <v>3.22</v>
-      </c>
-      <c r="M7">
-        <v>68.19</v>
-      </c>
-      <c r="N7">
-        <v>8.42</v>
-      </c>
-      <c r="O7">
-        <v>10.61</v>
-      </c>
-      <c r="P7">
-        <v>6.78</v>
-      </c>
-      <c r="Q7">
-        <v>400</v>
-      </c>
-      <c r="R7">
-        <v>400</v>
-      </c>
-      <c r="S7">
-        <v>400</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7">
-        <v>8610</v>
-      </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-      <c r="Z7">
-        <v>220</v>
-      </c>
-      <c r="AA7">
-        <v>12.21</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>16</v>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="G7" s="2">
+        <f>SUM(G2:G6)/5</f>
+        <v>3.9579999999999997</v>
+      </c>
+      <c r="N7" s="2">
+        <f>SUM(N2:N6)/5</f>
+        <v>5.0540000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>20</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>20</v>
       </c>
       <c r="E8">
-        <v>3.53</v>
+        <v>3.55</v>
       </c>
       <c r="F8">
-        <v>3.72</v>
+        <v>3.76</v>
       </c>
       <c r="G8">
-        <v>4.79</v>
+        <v>4.8</v>
       </c>
       <c r="H8">
-        <v>6.92</v>
+        <v>6.99</v>
       </c>
       <c r="I8">
-        <v>12.94</v>
+        <v>15.32</v>
       </c>
       <c r="J8">
-        <v>33.39</v>
+        <v>64.97</v>
       </c>
       <c r="K8">
-        <v>3.2</v>
+        <v>3.23</v>
       </c>
       <c r="L8">
-        <v>3.19</v>
+        <v>3.22</v>
       </c>
       <c r="M8">
-        <v>36.58</v>
+        <v>68.19</v>
       </c>
       <c r="N8">
+        <v>8.42</v>
+      </c>
+      <c r="O8">
+        <v>10.61</v>
+      </c>
+      <c r="P8">
         <v>6.78</v>
-      </c>
-      <c r="O8">
-        <v>5.56</v>
-      </c>
-      <c r="P8">
-        <v>5.36</v>
       </c>
       <c r="Q8">
         <v>400</v>
@@ -1333,66 +2454,66 @@
         <v>0</v>
       </c>
       <c r="Z8">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="AA8">
-        <v>12.11</v>
+        <v>12.21</v>
       </c>
       <c r="AB8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="AC8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>20</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>20</v>
       </c>
       <c r="E9">
-        <v>3.6</v>
+        <v>3.53</v>
       </c>
       <c r="F9">
-        <v>3.88</v>
+        <v>3.72</v>
       </c>
       <c r="G9">
-        <v>4.8099999999999996</v>
+        <v>4.79</v>
       </c>
       <c r="H9">
-        <v>7.22</v>
+        <v>6.92</v>
       </c>
       <c r="I9">
-        <v>12.92</v>
+        <v>12.94</v>
       </c>
       <c r="J9">
-        <v>55.44</v>
+        <v>33.39</v>
       </c>
       <c r="K9">
-        <v>3.34</v>
+        <v>3.2</v>
       </c>
       <c r="L9">
-        <v>2.98</v>
+        <v>3.19</v>
       </c>
       <c r="M9">
-        <v>58.41</v>
+        <v>36.58</v>
       </c>
       <c r="N9">
-        <v>7.91</v>
+        <v>6.78</v>
       </c>
       <c r="O9">
-        <v>9.5299999999999994</v>
+        <v>5.56</v>
       </c>
       <c r="P9">
-        <v>6.14</v>
+        <v>5.36</v>
       </c>
       <c r="Q9">
         <v>400</v>
@@ -1422,66 +2543,66 @@
         <v>0</v>
       </c>
       <c r="Z9">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="AA9">
-        <v>11.56</v>
+        <v>12.11</v>
       </c>
       <c r="AB9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AC9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>20</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>20</v>
       </c>
       <c r="E10">
-        <v>3.48</v>
+        <v>3.6</v>
       </c>
       <c r="F10">
-        <v>3.68</v>
+        <v>3.88</v>
       </c>
       <c r="G10">
-        <v>4.8499999999999996</v>
+        <v>4.8099999999999996</v>
       </c>
       <c r="H10">
-        <v>6.9</v>
+        <v>7.22</v>
       </c>
       <c r="I10">
-        <v>12.36</v>
+        <v>12.92</v>
       </c>
       <c r="J10">
-        <v>48.69</v>
+        <v>55.44</v>
       </c>
       <c r="K10">
-        <v>3.22</v>
+        <v>3.34</v>
       </c>
       <c r="L10">
-        <v>3.18</v>
+        <v>2.98</v>
       </c>
       <c r="M10">
-        <v>51.87</v>
+        <v>58.41</v>
       </c>
       <c r="N10">
-        <v>7.72</v>
+        <v>7.91</v>
       </c>
       <c r="O10">
-        <v>9.2100000000000009</v>
+        <v>9.5299999999999994</v>
       </c>
       <c r="P10">
-        <v>6.08</v>
+        <v>6.14</v>
       </c>
       <c r="Q10">
         <v>400</v>
@@ -1511,66 +2632,66 @@
         <v>0</v>
       </c>
       <c r="Z10">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="AA10">
-        <v>12.23</v>
+        <v>11.56</v>
       </c>
       <c r="AB10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AC10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>20</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>20</v>
       </c>
       <c r="E11">
-        <v>3.49</v>
+        <v>3.48</v>
       </c>
       <c r="F11">
-        <v>3.71</v>
+        <v>3.68</v>
       </c>
       <c r="G11">
-        <v>4.26</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="H11">
-        <v>6.54</v>
+        <v>6.9</v>
       </c>
       <c r="I11">
-        <v>10.1</v>
+        <v>12.36</v>
       </c>
       <c r="J11">
-        <v>48.61</v>
+        <v>48.69</v>
       </c>
       <c r="K11">
-        <v>2.83</v>
+        <v>3.22</v>
       </c>
       <c r="L11">
-        <v>3.13</v>
+        <v>3.18</v>
       </c>
       <c r="M11">
-        <v>51.74</v>
+        <v>51.87</v>
       </c>
       <c r="N11">
-        <v>7.07</v>
+        <v>7.72</v>
       </c>
       <c r="O11">
-        <v>8.33</v>
+        <v>9.2100000000000009</v>
       </c>
       <c r="P11">
-        <v>5.69</v>
+        <v>6.08</v>
       </c>
       <c r="Q11">
         <v>400</v>
@@ -1600,75 +2721,75 @@
         <v>0</v>
       </c>
       <c r="Z11">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="AA11">
-        <v>12.54</v>
+        <v>12.23</v>
       </c>
       <c r="AB11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AC11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C12">
-        <v>30</v>
-      </c>
-      <c r="D12">
+      <c r="C12" s="3">
         <v>20</v>
       </c>
+      <c r="D12" s="3">
+        <v>20</v>
+      </c>
       <c r="E12">
-        <v>4.83</v>
+        <v>3.49</v>
       </c>
       <c r="F12">
-        <v>5.3</v>
+        <v>3.71</v>
       </c>
       <c r="G12">
-        <v>6.95</v>
+        <v>4.26</v>
       </c>
       <c r="H12">
-        <v>10.67</v>
+        <v>6.54</v>
       </c>
       <c r="I12">
-        <v>19.12</v>
+        <v>10.1</v>
       </c>
       <c r="J12">
-        <v>115.4</v>
+        <v>48.61</v>
       </c>
       <c r="K12">
-        <v>5.37</v>
+        <v>2.83</v>
       </c>
       <c r="L12">
-        <v>4.3099999999999996</v>
+        <v>3.13</v>
       </c>
       <c r="M12">
-        <v>119.7</v>
+        <v>51.74</v>
       </c>
       <c r="N12">
-        <v>13</v>
+        <v>7.07</v>
       </c>
       <c r="O12">
-        <v>19.649999999999999</v>
+        <v>8.33</v>
       </c>
       <c r="P12">
-        <v>11.25</v>
+        <v>5.69</v>
       </c>
       <c r="Q12">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="R12">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="S12">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="T12">
         <v>0</v>
@@ -1677,7 +2798,7 @@
         <v>0</v>
       </c>
       <c r="V12">
-        <v>19365</v>
+        <v>8610</v>
       </c>
       <c r="W12">
         <v>0</v>
@@ -1689,155 +2810,80 @@
         <v>0</v>
       </c>
       <c r="Z12">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="AA12">
-        <v>12.95</v>
+        <v>12.54</v>
       </c>
       <c r="AB12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AC12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>30</v>
-      </c>
-      <c r="D13">
-        <v>20</v>
-      </c>
-      <c r="E13">
-        <v>4.8499999999999996</v>
-      </c>
-      <c r="F13">
-        <v>5.25</v>
-      </c>
-      <c r="G13">
-        <v>6.7</v>
-      </c>
-      <c r="H13">
-        <v>11.11</v>
-      </c>
-      <c r="I13">
-        <v>19.5</v>
-      </c>
-      <c r="J13">
-        <v>99.37</v>
-      </c>
-      <c r="K13">
-        <v>5.85</v>
-      </c>
-      <c r="L13">
-        <v>4.3600000000000003</v>
-      </c>
-      <c r="M13">
-        <v>103.73</v>
-      </c>
-      <c r="N13">
-        <v>12.61</v>
-      </c>
-      <c r="O13">
-        <v>18.260000000000002</v>
-      </c>
-      <c r="P13">
-        <v>10.7</v>
-      </c>
-      <c r="Q13">
-        <v>600</v>
-      </c>
-      <c r="R13">
-        <v>600</v>
-      </c>
-      <c r="S13">
-        <v>600</v>
-      </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
-      <c r="U13">
-        <v>0</v>
-      </c>
-      <c r="V13">
-        <v>19365</v>
-      </c>
-      <c r="W13">
-        <v>0</v>
-      </c>
-      <c r="X13">
-        <v>0</v>
-      </c>
-      <c r="Y13">
-        <v>0</v>
-      </c>
-      <c r="Z13">
-        <v>254</v>
-      </c>
-      <c r="AA13">
-        <v>12.17</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>28</v>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="G13" s="2">
+        <f>SUM(G8:G12)/5</f>
+        <v>4.702</v>
+      </c>
+      <c r="N13" s="2">
+        <f>SUM(N8:N12)/5</f>
+        <v>7.58</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
         <v>30</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="3">
         <v>20</v>
       </c>
       <c r="E14">
-        <v>4.87</v>
+        <v>4.83</v>
       </c>
       <c r="F14">
-        <v>5.4</v>
+        <v>5.3</v>
       </c>
       <c r="G14">
-        <v>7.46</v>
+        <v>6.95</v>
       </c>
       <c r="H14">
-        <v>10.82</v>
+        <v>10.67</v>
       </c>
       <c r="I14">
-        <v>21.9</v>
+        <v>19.12</v>
       </c>
       <c r="J14">
-        <v>120.01</v>
+        <v>115.4</v>
       </c>
       <c r="K14">
-        <v>5.42</v>
+        <v>5.37</v>
       </c>
       <c r="L14">
-        <v>4.22</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="M14">
-        <v>124.23</v>
+        <v>119.7</v>
       </c>
       <c r="N14">
-        <v>13.29</v>
+        <v>13</v>
       </c>
       <c r="O14">
-        <v>20.07</v>
+        <v>19.649999999999999</v>
       </c>
       <c r="P14">
-        <v>11.42</v>
+        <v>11.25</v>
       </c>
       <c r="Q14">
         <v>600</v>
@@ -1867,66 +2913,66 @@
         <v>0</v>
       </c>
       <c r="Z14">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="AA14">
-        <v>12.36</v>
+        <v>12.95</v>
       </c>
       <c r="AB14" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="AC14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <v>30</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>20</v>
       </c>
       <c r="E15">
-        <v>4.8099999999999996</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="F15">
-        <v>5.29</v>
+        <v>5.25</v>
       </c>
       <c r="G15">
-        <v>7.03</v>
+        <v>6.7</v>
       </c>
       <c r="H15">
-        <v>10.61</v>
+        <v>11.11</v>
       </c>
       <c r="I15">
-        <v>18.37</v>
+        <v>19.5</v>
       </c>
       <c r="J15">
-        <v>124.63</v>
+        <v>99.37</v>
       </c>
       <c r="K15">
-        <v>5.32</v>
+        <v>5.85</v>
       </c>
       <c r="L15">
-        <v>4.1399999999999997</v>
+        <v>4.3600000000000003</v>
       </c>
       <c r="M15">
-        <v>128.77000000000001</v>
+        <v>103.73</v>
       </c>
       <c r="N15">
-        <v>13.54</v>
+        <v>12.61</v>
       </c>
       <c r="O15">
-        <v>23.04</v>
+        <v>18.260000000000002</v>
       </c>
       <c r="P15">
-        <v>12</v>
+        <v>10.7</v>
       </c>
       <c r="Q15">
         <v>600</v>
@@ -1956,66 +3002,66 @@
         <v>0</v>
       </c>
       <c r="Z15">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="AA15">
-        <v>12.56</v>
+        <v>12.17</v>
       </c>
       <c r="AB15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="AC15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <v>30</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <v>20</v>
       </c>
       <c r="E16">
-        <v>4.8099999999999996</v>
+        <v>4.87</v>
       </c>
       <c r="F16">
-        <v>5.24</v>
+        <v>5.4</v>
       </c>
       <c r="G16">
-        <v>7.47</v>
+        <v>7.46</v>
       </c>
       <c r="H16">
-        <v>10.53</v>
+        <v>10.82</v>
       </c>
       <c r="I16">
-        <v>18.850000000000001</v>
+        <v>21.9</v>
       </c>
       <c r="J16">
-        <v>73.61</v>
+        <v>120.01</v>
       </c>
       <c r="K16">
-        <v>5.29</v>
+        <v>5.42</v>
       </c>
       <c r="L16">
-        <v>4.01</v>
+        <v>4.22</v>
       </c>
       <c r="M16">
-        <v>77.61</v>
+        <v>124.23</v>
       </c>
       <c r="N16">
-        <v>11.22</v>
+        <v>13.29</v>
       </c>
       <c r="O16">
-        <v>12.39</v>
+        <v>20.07</v>
       </c>
       <c r="P16">
-        <v>9.4600000000000009</v>
+        <v>11.42</v>
       </c>
       <c r="Q16">
         <v>600</v>
@@ -2045,75 +3091,75 @@
         <v>0</v>
       </c>
       <c r="Z16">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="AA16">
-        <v>12.96</v>
+        <v>12.36</v>
       </c>
       <c r="AB16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="AC16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C17">
-        <v>40</v>
-      </c>
-      <c r="D17">
+      <c r="C17" s="3">
+        <v>30</v>
+      </c>
+      <c r="D17" s="3">
         <v>20</v>
       </c>
       <c r="E17">
-        <v>6.06</v>
+        <v>4.8099999999999996</v>
       </c>
       <c r="F17">
-        <v>6.56</v>
+        <v>5.29</v>
       </c>
       <c r="G17">
-        <v>8.7799999999999994</v>
+        <v>7.03</v>
       </c>
       <c r="H17">
-        <v>14.68</v>
+        <v>10.61</v>
       </c>
       <c r="I17">
-        <v>25.46</v>
+        <v>18.37</v>
       </c>
       <c r="J17">
-        <v>140.16999999999999</v>
+        <v>124.63</v>
       </c>
       <c r="K17">
-        <v>8.1300000000000008</v>
+        <v>5.32</v>
       </c>
       <c r="L17">
-        <v>5.0199999999999996</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="M17">
-        <v>145.19999999999999</v>
+        <v>128.77000000000001</v>
       </c>
       <c r="N17">
-        <v>16.690000000000001</v>
+        <v>13.54</v>
       </c>
       <c r="O17">
-        <v>25.5</v>
+        <v>23.04</v>
       </c>
       <c r="P17">
-        <v>14.65</v>
+        <v>12</v>
       </c>
       <c r="Q17">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="R17">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="S17">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="T17">
         <v>0</v>
@@ -2122,7 +3168,7 @@
         <v>0</v>
       </c>
       <c r="V17">
-        <v>34420</v>
+        <v>19365</v>
       </c>
       <c r="W17">
         <v>0</v>
@@ -2134,75 +3180,75 @@
         <v>0</v>
       </c>
       <c r="Z17">
-        <v>330</v>
+        <v>269</v>
       </c>
       <c r="AA17">
-        <v>12.45</v>
+        <v>12.56</v>
       </c>
       <c r="AB17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AC17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C18">
-        <v>40</v>
-      </c>
-      <c r="D18">
+      <c r="C18" s="3">
+        <v>30</v>
+      </c>
+      <c r="D18" s="3">
         <v>20</v>
       </c>
       <c r="E18">
-        <v>6.11</v>
+        <v>4.8099999999999996</v>
       </c>
       <c r="F18">
-        <v>6.62</v>
+        <v>5.24</v>
       </c>
       <c r="G18">
-        <v>8.68</v>
+        <v>7.47</v>
       </c>
       <c r="H18">
-        <v>13.68</v>
+        <v>10.53</v>
       </c>
       <c r="I18">
-        <v>22.88</v>
+        <v>18.850000000000001</v>
       </c>
       <c r="J18">
-        <v>149.79</v>
+        <v>73.61</v>
       </c>
       <c r="K18">
-        <v>7.06</v>
+        <v>5.29</v>
       </c>
       <c r="L18">
-        <v>5.23</v>
+        <v>4.01</v>
       </c>
       <c r="M18">
-        <v>155.01</v>
+        <v>77.61</v>
       </c>
       <c r="N18">
-        <v>14.77</v>
+        <v>11.22</v>
       </c>
       <c r="O18">
-        <v>20.03</v>
+        <v>12.39</v>
       </c>
       <c r="P18">
-        <v>13</v>
+        <v>9.4600000000000009</v>
       </c>
       <c r="Q18">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="R18">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="S18">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="T18">
         <v>0</v>
@@ -2211,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="V18">
-        <v>34420</v>
+        <v>19365</v>
       </c>
       <c r="W18">
         <v>0</v>
@@ -2223,155 +3269,80 @@
         <v>0</v>
       </c>
       <c r="Z18">
-        <v>329</v>
+        <v>275</v>
       </c>
       <c r="AA18">
-        <v>12.21</v>
+        <v>12.96</v>
       </c>
       <c r="AB18" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="AC18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19">
-        <v>40</v>
-      </c>
-      <c r="D19">
-        <v>20</v>
-      </c>
-      <c r="E19">
-        <v>6.17</v>
-      </c>
-      <c r="F19">
-        <v>6.85</v>
-      </c>
-      <c r="G19">
-        <v>9.77</v>
-      </c>
-      <c r="H19">
-        <v>16.29</v>
-      </c>
-      <c r="I19">
-        <v>27.52</v>
-      </c>
-      <c r="J19">
-        <v>139.91</v>
-      </c>
-      <c r="K19">
-        <v>9.44</v>
-      </c>
-      <c r="L19">
-        <v>5.27</v>
-      </c>
-      <c r="M19">
-        <v>145.19</v>
-      </c>
-      <c r="N19">
-        <v>16.41</v>
-      </c>
-      <c r="O19">
-        <v>20.74</v>
-      </c>
-      <c r="P19">
-        <v>14.51</v>
-      </c>
-      <c r="Q19">
-        <v>800</v>
-      </c>
-      <c r="R19">
-        <v>800</v>
-      </c>
-      <c r="S19">
-        <v>800</v>
-      </c>
-      <c r="T19">
-        <v>0</v>
-      </c>
-      <c r="U19">
-        <v>0</v>
-      </c>
-      <c r="V19">
-        <v>34420</v>
-      </c>
-      <c r="W19">
-        <v>0</v>
-      </c>
-      <c r="X19">
-        <v>0</v>
-      </c>
-      <c r="Y19">
-        <v>0</v>
-      </c>
-      <c r="Z19">
-        <v>329</v>
-      </c>
-      <c r="AA19">
-        <v>12.31</v>
-      </c>
-      <c r="AB19" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC19" t="s">
-        <v>40</v>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="G19" s="2">
+        <f>SUM(G14:G18)/5</f>
+        <v>7.1219999999999999</v>
+      </c>
+      <c r="N19" s="2">
+        <f>SUM(N14:N18)/5</f>
+        <v>12.731999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="3">
         <v>40</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
         <v>20</v>
       </c>
       <c r="E20">
-        <v>6.04</v>
+        <v>6.06</v>
       </c>
       <c r="F20">
-        <v>6.73</v>
+        <v>6.56</v>
       </c>
       <c r="G20">
-        <v>9.34</v>
+        <v>8.7799999999999994</v>
       </c>
       <c r="H20">
-        <v>15.14</v>
+        <v>14.68</v>
       </c>
       <c r="I20">
-        <v>29.29</v>
+        <v>25.46</v>
       </c>
       <c r="J20">
-        <v>133.81</v>
+        <v>140.16999999999999</v>
       </c>
       <c r="K20">
-        <v>8.42</v>
+        <v>8.1300000000000008</v>
       </c>
       <c r="L20">
-        <v>5.19</v>
+        <v>5.0199999999999996</v>
       </c>
       <c r="M20">
-        <v>139.01</v>
+        <v>145.19999999999999</v>
       </c>
       <c r="N20">
-        <v>16.28</v>
+        <v>16.690000000000001</v>
       </c>
       <c r="O20">
-        <v>21.23</v>
+        <v>25.5</v>
       </c>
       <c r="P20">
-        <v>14.35</v>
+        <v>14.65</v>
       </c>
       <c r="Q20">
         <v>800</v>
@@ -2404,63 +3375,63 @@
         <v>330</v>
       </c>
       <c r="AA20">
-        <v>12.91</v>
+        <v>12.45</v>
       </c>
       <c r="AB20" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="AC20" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="3">
         <v>40</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="3">
         <v>20</v>
       </c>
       <c r="E21">
-        <v>6.15</v>
+        <v>6.11</v>
       </c>
       <c r="F21">
-        <v>6.86</v>
+        <v>6.62</v>
       </c>
       <c r="G21">
-        <v>9.15</v>
+        <v>8.68</v>
       </c>
       <c r="H21">
-        <v>15.02</v>
+        <v>13.68</v>
       </c>
       <c r="I21">
-        <v>23.37</v>
+        <v>22.88</v>
       </c>
       <c r="J21">
-        <v>129.19999999999999</v>
+        <v>149.79</v>
       </c>
       <c r="K21">
-        <v>8.17</v>
+        <v>7.06</v>
       </c>
       <c r="L21">
-        <v>5.13</v>
+        <v>5.23</v>
       </c>
       <c r="M21">
-        <v>134.33000000000001</v>
+        <v>155.01</v>
       </c>
       <c r="N21">
-        <v>16.010000000000002</v>
+        <v>14.77</v>
       </c>
       <c r="O21">
-        <v>22.12</v>
+        <v>20.03</v>
       </c>
       <c r="P21">
-        <v>14.32</v>
+        <v>13</v>
       </c>
       <c r="Q21">
         <v>800</v>
@@ -2493,72 +3464,72 @@
         <v>329</v>
       </c>
       <c r="AA21">
-        <v>11.82</v>
+        <v>12.21</v>
       </c>
       <c r="AB21" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="AC21" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C22">
-        <v>50</v>
-      </c>
-      <c r="D22">
+      <c r="C22" s="3">
+        <v>40</v>
+      </c>
+      <c r="D22" s="3">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>8.0399999999999991</v>
+        <v>6.17</v>
       </c>
       <c r="F22">
-        <v>9.82</v>
+        <v>6.85</v>
       </c>
       <c r="G22">
-        <v>14.79</v>
+        <v>9.77</v>
       </c>
       <c r="H22">
-        <v>24.75</v>
+        <v>16.29</v>
       </c>
       <c r="I22">
-        <v>43.23</v>
+        <v>27.52</v>
       </c>
       <c r="J22">
-        <v>189.35</v>
+        <v>139.91</v>
       </c>
       <c r="K22">
-        <v>14.93</v>
+        <v>9.44</v>
       </c>
       <c r="L22">
-        <v>6.49</v>
+        <v>5.27</v>
       </c>
       <c r="M22">
-        <v>195.84</v>
+        <v>145.19</v>
       </c>
       <c r="N22">
-        <v>25.01</v>
+        <v>16.41</v>
       </c>
       <c r="O22">
-        <v>32.29</v>
+        <v>20.74</v>
       </c>
       <c r="P22">
-        <v>22.31</v>
+        <v>14.51</v>
       </c>
       <c r="Q22">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="R22">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="S22">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="T22">
         <v>0</v>
@@ -2567,7 +3538,7 @@
         <v>0</v>
       </c>
       <c r="V22">
-        <v>53775</v>
+        <v>34420</v>
       </c>
       <c r="W22">
         <v>0</v>
@@ -2579,75 +3550,75 @@
         <v>0</v>
       </c>
       <c r="Z22">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AA22">
-        <v>12.48</v>
+        <v>12.31</v>
       </c>
       <c r="AB22" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="AC22" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C23">
-        <v>50</v>
-      </c>
-      <c r="D23">
+      <c r="C23" s="3">
+        <v>40</v>
+      </c>
+      <c r="D23" s="3">
         <v>20</v>
       </c>
       <c r="E23">
-        <v>7.9</v>
+        <v>6.04</v>
       </c>
       <c r="F23">
-        <v>9.69</v>
+        <v>6.73</v>
       </c>
       <c r="G23">
-        <v>14.97</v>
+        <v>9.34</v>
       </c>
       <c r="H23">
-        <v>24.05</v>
+        <v>15.14</v>
       </c>
       <c r="I23">
-        <v>43.41</v>
+        <v>29.29</v>
       </c>
       <c r="J23">
-        <v>223.56</v>
+        <v>133.81</v>
       </c>
       <c r="K23">
-        <v>14.37</v>
+        <v>8.42</v>
       </c>
       <c r="L23">
-        <v>6.5</v>
+        <v>5.19</v>
       </c>
       <c r="M23">
-        <v>230.06</v>
+        <v>139.01</v>
       </c>
       <c r="N23">
-        <v>25.13</v>
+        <v>16.28</v>
       </c>
       <c r="O23">
-        <v>33.700000000000003</v>
+        <v>21.23</v>
       </c>
       <c r="P23">
-        <v>22.92</v>
+        <v>14.35</v>
       </c>
       <c r="Q23">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="R23">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="S23">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="T23">
         <v>0</v>
@@ -2656,7 +3627,7 @@
         <v>0</v>
       </c>
       <c r="V23">
-        <v>53775</v>
+        <v>34420</v>
       </c>
       <c r="W23">
         <v>0</v>
@@ -2668,75 +3639,75 @@
         <v>0</v>
       </c>
       <c r="Z23">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="AA23">
-        <v>12.51</v>
+        <v>12.91</v>
       </c>
       <c r="AB23" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AC23" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C24">
-        <v>50</v>
-      </c>
-      <c r="D24">
+      <c r="C24" s="3">
+        <v>40</v>
+      </c>
+      <c r="D24" s="3">
         <v>20</v>
       </c>
       <c r="E24">
-        <v>7.73</v>
+        <v>6.15</v>
       </c>
       <c r="F24">
-        <v>9.35</v>
+        <v>6.86</v>
       </c>
       <c r="G24">
-        <v>14.29</v>
+        <v>9.15</v>
       </c>
       <c r="H24">
-        <v>22.99</v>
+        <v>15.02</v>
       </c>
       <c r="I24">
-        <v>37.4</v>
+        <v>23.37</v>
       </c>
       <c r="J24">
-        <v>200.93</v>
+        <v>129.19999999999999</v>
       </c>
       <c r="K24">
-        <v>13.65</v>
+        <v>8.17</v>
       </c>
       <c r="L24">
-        <v>6.31</v>
+        <v>5.13</v>
       </c>
       <c r="M24">
-        <v>207.24</v>
+        <v>134.33000000000001</v>
       </c>
       <c r="N24">
-        <v>23.27</v>
+        <v>16.010000000000002</v>
       </c>
       <c r="O24">
-        <v>30.93</v>
+        <v>22.12</v>
       </c>
       <c r="P24">
-        <v>20.88</v>
+        <v>14.32</v>
       </c>
       <c r="Q24">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="R24">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="S24">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="T24">
         <v>0</v>
@@ -2745,7 +3716,7 @@
         <v>0</v>
       </c>
       <c r="V24">
-        <v>53775</v>
+        <v>34420</v>
       </c>
       <c r="W24">
         <v>0</v>
@@ -2757,155 +3728,80 @@
         <v>0</v>
       </c>
       <c r="Z24">
-        <v>351</v>
+        <v>329</v>
       </c>
       <c r="AA24">
-        <v>12.19</v>
+        <v>11.82</v>
       </c>
       <c r="AB24" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="AC24" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25">
-        <v>50</v>
-      </c>
-      <c r="D25">
-        <v>20</v>
-      </c>
-      <c r="E25">
-        <v>7.59</v>
-      </c>
-      <c r="F25">
-        <v>8.9</v>
-      </c>
-      <c r="G25">
-        <v>13.59</v>
-      </c>
-      <c r="H25">
-        <v>21.37</v>
-      </c>
-      <c r="I25">
-        <v>35.35</v>
-      </c>
-      <c r="J25">
-        <v>171.79</v>
-      </c>
-      <c r="K25">
-        <v>12.48</v>
-      </c>
-      <c r="L25">
-        <v>6.13</v>
-      </c>
-      <c r="M25">
-        <v>177.91</v>
-      </c>
-      <c r="N25">
-        <v>22.33</v>
-      </c>
-      <c r="O25">
-        <v>30.44</v>
-      </c>
-      <c r="P25">
-        <v>20.09</v>
-      </c>
-      <c r="Q25">
-        <v>1000</v>
-      </c>
-      <c r="R25">
-        <v>1000</v>
-      </c>
-      <c r="S25">
-        <v>1000</v>
-      </c>
-      <c r="T25">
-        <v>0</v>
-      </c>
-      <c r="U25">
-        <v>0</v>
-      </c>
-      <c r="V25">
-        <v>53775</v>
-      </c>
-      <c r="W25">
-        <v>0</v>
-      </c>
-      <c r="X25">
-        <v>0</v>
-      </c>
-      <c r="Y25">
-        <v>0</v>
-      </c>
-      <c r="Z25">
-        <v>368</v>
-      </c>
-      <c r="AA25">
-        <v>12.56</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC25" t="s">
-        <v>52</v>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="G25" s="2">
+        <f>SUM(G20:G24)/5</f>
+        <v>9.1440000000000001</v>
+      </c>
+      <c r="N25" s="2">
+        <f>SUM(N20:N24)/5</f>
+        <v>16.032000000000004</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="A26" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="3">
         <v>50</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="3">
         <v>20</v>
       </c>
       <c r="E26">
-        <v>7.65</v>
+        <v>8.0399999999999991</v>
       </c>
       <c r="F26">
-        <v>8.9600000000000009</v>
+        <v>9.82</v>
       </c>
       <c r="G26">
-        <v>13.44</v>
+        <v>14.79</v>
       </c>
       <c r="H26">
-        <v>22.4</v>
+        <v>24.75</v>
       </c>
       <c r="I26">
-        <v>37.880000000000003</v>
+        <v>43.23</v>
       </c>
       <c r="J26">
-        <v>179.24</v>
+        <v>189.35</v>
       </c>
       <c r="K26">
-        <v>13.44</v>
+        <v>14.93</v>
       </c>
       <c r="L26">
-        <v>6.32</v>
+        <v>6.49</v>
       </c>
       <c r="M26">
-        <v>185.56</v>
+        <v>195.84</v>
       </c>
       <c r="N26">
-        <v>22.58</v>
+        <v>25.01</v>
       </c>
       <c r="O26">
-        <v>28.99</v>
+        <v>32.29</v>
       </c>
       <c r="P26">
-        <v>20.49</v>
+        <v>22.31</v>
       </c>
       <c r="Q26">
         <v>1000</v>
@@ -2935,20 +3831,425 @@
         <v>0</v>
       </c>
       <c r="Z26">
+        <v>328</v>
+      </c>
+      <c r="AA26">
+        <v>12.48</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="3">
+        <v>50</v>
+      </c>
+      <c r="D27" s="3">
+        <v>20</v>
+      </c>
+      <c r="E27">
+        <v>7.9</v>
+      </c>
+      <c r="F27">
+        <v>9.69</v>
+      </c>
+      <c r="G27">
+        <v>14.97</v>
+      </c>
+      <c r="H27">
+        <v>24.05</v>
+      </c>
+      <c r="I27">
+        <v>43.41</v>
+      </c>
+      <c r="J27">
+        <v>223.56</v>
+      </c>
+      <c r="K27">
+        <v>14.37</v>
+      </c>
+      <c r="L27">
+        <v>6.5</v>
+      </c>
+      <c r="M27">
+        <v>230.06</v>
+      </c>
+      <c r="N27">
+        <v>25.13</v>
+      </c>
+      <c r="O27">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="P27">
+        <v>22.92</v>
+      </c>
+      <c r="Q27">
+        <v>1000</v>
+      </c>
+      <c r="R27">
+        <v>1000</v>
+      </c>
+      <c r="S27">
+        <v>1000</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>53775</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>339</v>
+      </c>
+      <c r="AA27">
+        <v>12.51</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="3">
+        <v>50</v>
+      </c>
+      <c r="D28" s="3">
+        <v>20</v>
+      </c>
+      <c r="E28">
+        <v>7.73</v>
+      </c>
+      <c r="F28">
+        <v>9.35</v>
+      </c>
+      <c r="G28">
+        <v>14.29</v>
+      </c>
+      <c r="H28">
+        <v>22.99</v>
+      </c>
+      <c r="I28">
+        <v>37.4</v>
+      </c>
+      <c r="J28">
+        <v>200.93</v>
+      </c>
+      <c r="K28">
+        <v>13.65</v>
+      </c>
+      <c r="L28">
+        <v>6.31</v>
+      </c>
+      <c r="M28">
+        <v>207.24</v>
+      </c>
+      <c r="N28">
+        <v>23.27</v>
+      </c>
+      <c r="O28">
+        <v>30.93</v>
+      </c>
+      <c r="P28">
+        <v>20.88</v>
+      </c>
+      <c r="Q28">
+        <v>1000</v>
+      </c>
+      <c r="R28">
+        <v>1000</v>
+      </c>
+      <c r="S28">
+        <v>1000</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>53775</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <v>351</v>
+      </c>
+      <c r="AA28">
+        <v>12.19</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="3">
+        <v>50</v>
+      </c>
+      <c r="D29" s="3">
+        <v>20</v>
+      </c>
+      <c r="E29">
+        <v>7.59</v>
+      </c>
+      <c r="F29">
+        <v>8.9</v>
+      </c>
+      <c r="G29">
+        <v>13.59</v>
+      </c>
+      <c r="H29">
+        <v>21.37</v>
+      </c>
+      <c r="I29">
+        <v>35.35</v>
+      </c>
+      <c r="J29">
+        <v>171.79</v>
+      </c>
+      <c r="K29">
+        <v>12.48</v>
+      </c>
+      <c r="L29">
+        <v>6.13</v>
+      </c>
+      <c r="M29">
+        <v>177.91</v>
+      </c>
+      <c r="N29">
+        <v>22.33</v>
+      </c>
+      <c r="O29">
+        <v>30.44</v>
+      </c>
+      <c r="P29">
+        <v>20.09</v>
+      </c>
+      <c r="Q29">
+        <v>1000</v>
+      </c>
+      <c r="R29">
+        <v>1000</v>
+      </c>
+      <c r="S29">
+        <v>1000</v>
+      </c>
+      <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <v>53775</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
+      <c r="Y29">
+        <v>0</v>
+      </c>
+      <c r="Z29">
+        <v>368</v>
+      </c>
+      <c r="AA29">
+        <v>12.56</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="3">
+        <v>50</v>
+      </c>
+      <c r="D30" s="3">
+        <v>20</v>
+      </c>
+      <c r="E30">
+        <v>7.65</v>
+      </c>
+      <c r="F30">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="G30">
+        <v>13.44</v>
+      </c>
+      <c r="H30">
+        <v>22.4</v>
+      </c>
+      <c r="I30">
+        <v>37.880000000000003</v>
+      </c>
+      <c r="J30">
+        <v>179.24</v>
+      </c>
+      <c r="K30">
+        <v>13.44</v>
+      </c>
+      <c r="L30">
+        <v>6.32</v>
+      </c>
+      <c r="M30">
+        <v>185.56</v>
+      </c>
+      <c r="N30">
+        <v>22.58</v>
+      </c>
+      <c r="O30">
+        <v>28.99</v>
+      </c>
+      <c r="P30">
+        <v>20.49</v>
+      </c>
+      <c r="Q30">
+        <v>1000</v>
+      </c>
+      <c r="R30">
+        <v>1000</v>
+      </c>
+      <c r="S30">
+        <v>1000</v>
+      </c>
+      <c r="T30">
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <v>53775</v>
+      </c>
+      <c r="W30">
+        <v>0</v>
+      </c>
+      <c r="X30">
+        <v>0</v>
+      </c>
+      <c r="Y30">
+        <v>0</v>
+      </c>
+      <c r="Z30">
         <v>386</v>
       </c>
-      <c r="AA26">
+      <c r="AA30">
         <v>12.25</v>
       </c>
-      <c r="AB26" t="s">
+      <c r="AB30" t="s">
         <v>53</v>
       </c>
-      <c r="AC26" t="s">
+      <c r="AC30" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="G31" s="2">
+        <f>SUM(G26:G30)/5</f>
+        <v>14.215999999999999</v>
+      </c>
+      <c r="N31" s="2">
+        <f>SUM(N26:N30)/5</f>
+        <v>23.663999999999998</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
+  <mergeCells count="20">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="D14:D18"/>
+    <mergeCell ref="D20:D24"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="C20:C24"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="B2:B6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EEDAB26-B4B7-1644-ABBC-375B0C0E392B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>